<commit_message>
chore: populating publication data with 2025 publications
</commit_message>
<xml_diff>
--- a/public/data/info.xlsx
+++ b/public/data/info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\pedro\Ciampitti_Lab\ciampitti-lab.github.io\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0880724E-3BCB-4DB4-AFC5-0B79C28A7179}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAE9B87-34BF-4860-BDA9-2301C5EC7C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="57">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="105">
   <si>
     <t>role</t>
   </si>
@@ -127,12 +127,6 @@
     <t>year</t>
   </si>
   <si>
-    <t>AVYield</t>
-  </si>
-  <si>
-    <t>Me Myself and I</t>
-  </si>
-  <si>
     <t>Postdoc</t>
   </si>
   <si>
@@ -205,10 +199,160 @@
     <t>md_file_name</t>
   </si>
   <si>
-    <t>test123</t>
-  </si>
-  <si>
-    <t>Computers and electronics in Agriculture</t>
+    <t>Nitrogen nutrition index as an in-season N diagnostic method for maize yield response to N fertilization</t>
+  </si>
+  <si>
+    <t>Leonardo Bosche, Federico Gomez, Francisco Palmero, Aidan Kerns, Trevor Hefley, Curtis Ransom, PV Vara Prasad, Bradley Van De Woestyne, Ignacio Ciampitti</t>
+  </si>
+  <si>
+    <t>Field Crops Research</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.fcr.2025.109941</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0378429025002060</t>
+  </si>
+  <si>
+    <t>A global dataset on mungbean for managing seed yield and quality</t>
+  </si>
+  <si>
+    <t>Natalia da Silva Volpato, Federico M Gomez, Víctor D Giménez, Ignacio A Ciampitti</t>
+  </si>
+  <si>
+    <t>Scientific Data</t>
+  </si>
+  <si>
+    <t>https://www.nature.com/articles/s41597-025-05016-6</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1038/s41597-025-05016-6</t>
+  </si>
+  <si>
+    <t>Spatio-temporal yield variation and precipitation within a field</t>
+  </si>
+  <si>
+    <t>Emmanuela van Versendaal, Carlos M Hernandez, Peter Kyveryga, Trevor Hefley, Bradley W Van De Woestyne, PV Vara Prasad, Ignacio A Ciampitti</t>
+  </si>
+  <si>
+    <t>Computers and Electronics in Agriculture</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.compag.2025.109996</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0168169925001024</t>
+  </si>
+  <si>
+    <t>A digital interactive decision dashboard for crop yield trials</t>
+  </si>
+  <si>
+    <t>Pedro Cisdeli, Gustavo Nocera Santiago, Carlos Hernandez, Ana Carcedo, PV Vara Prasad, Michael Stamm, Jane Lingenfelser, Ignacio Ciampitti</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0168169925001437</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.compag.2025.110037</t>
+  </si>
+  <si>
+    <t>Towards site-specific nutrient management strategies: An open database in Senegal</t>
+  </si>
+  <si>
+    <t>Federico Gomez, Ana Carcedo, Andre Diatta, Pape Djighaly, Latha Nagarajan, Upendra Singh, Zachary Stewart, Shamie Zingore, Kaushik Majumdar, PV Vara Prasad, Ignacio Ciampitti</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0048969725005613</t>
+  </si>
+  <si>
+    <t>Science of The Total Environment</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.scitotenv.2025.178926</t>
+  </si>
+  <si>
+    <t>Francisco Palmero, Javier A Fernandez, Jeffrey E Habben, Jeffrey R Schussler, Ben Weers, James Bing, Trevor Hefley, PV Vara Prasad, Ignacio A Ciampitti</t>
+  </si>
+  <si>
+    <t>DP202216 maize hybrids shift upper limit of C and N partitioning to grain</t>
+  </si>
+  <si>
+    <t>Frontiers in Plant Science</t>
+  </si>
+  <si>
+    <t>https://www.frontiersin.org/journals/plant-science/articles/10.3389/fpls.2025.1459126/full</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.3389/fpls.2025.1459126</t>
+  </si>
+  <si>
+    <t>Benchmarking sorghum and maize for both yield and economic advantage in the US Great Plains</t>
+  </si>
+  <si>
+    <t>Federico Gomez, Juan Manuel Sanchis, Víctor Giménez, Jane Lingenfelser, Ana Carcedo, Ignacio Massigoge, PV Vara Prasad, Ignacio Ciampitti</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0378429025000346</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.fcr.2025.109769</t>
+  </si>
+  <si>
+    <t>An in‐silico approach exploring sorghum source: sink balance across sorghum hybrids: How many leaves are enough?</t>
+  </si>
+  <si>
+    <t>Lucia Marziotte, Ana JP Carcedo, Laura Mayor, PV Vara Prasad, Joaquín A Peraza, Ignacio A Ciampitti</t>
+  </si>
+  <si>
+    <t>Crop Science</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/csc2.21449</t>
+  </si>
+  <si>
+    <t>https://acsess.onlinelibrary.wiley.com/doi/10.1002/csc2.21449</t>
+  </si>
+  <si>
+    <t>Assessing the influence of environmental drivers on soybean seed yield and nitrogen fixation estimates and uncertainties in the United States</t>
+  </si>
+  <si>
+    <t>Luiz Felipe Almeida, Adrian A Correndo, Trevor Hefley, Gabriel Hintz, PV Vara Prasad, Mark Licht, Shaun Casteel, Maninder Singh, Seth Naeve, José Bais, Laura Lindsay, Shawn Conley, Jonathan Kleinjan, Péter Kovács, Ignacio A Ciampitti</t>
+  </si>
+  <si>
+    <t>European Journal of Agronomy</t>
+  </si>
+  <si>
+    <t>Soybean yield and seed quality in equidistant versus non‐equidistant plant arrangements under different densities</t>
+  </si>
+  <si>
+    <t>Emmanuela van Versendaal, Valentina M Pereyra, Trent Irby, Peter Kovacs, Trevor Hefley, PV Vara Prasad, Peter Kyveryga, Bradley W Van De Woestyne, Ignacio A Ciampitti</t>
+  </si>
+  <si>
+    <t>Climate-adaptative management strategies for soybean production under ENSO scenarios in Southern Brazil: An in-silico analysis of crop failure risk</t>
+  </si>
+  <si>
+    <t>Gabriel Hintz, Ana Carcedo, Luiz Felipe Almeida, Geomar Corassa, Tiago Horbe, Luan Pott, Raí Schwalbert, Trevor Hefley, PV Vara Prasad, Ignacio Ciampitti</t>
+  </si>
+  <si>
+    <t>Agricultural Systems</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.agsy.2024.104153</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S0308521X24003032</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1002/csc2.21364</t>
+  </si>
+  <si>
+    <t>https://acsess.onlinelibrary.wiley.com/doi/full/10.1002/csc2.21364</t>
+  </si>
+  <si>
+    <t>https://doi.org/10.1016/j.eja.2024.127428</t>
+  </si>
+  <si>
+    <t>https://www.sciencedirect.com/science/article/abs/pii/S1161030124003496</t>
   </si>
 </sst>
 </file>
@@ -253,9 +397,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -618,10 +763,10 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E1" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
@@ -635,13 +780,13 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F2" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.25">
@@ -655,10 +800,10 @@
         <v>1</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F3" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.25">
@@ -672,10 +817,10 @@
         <v>2</v>
       </c>
       <c r="E4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -689,10 +834,10 @@
         <v>2</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F5" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -706,10 +851,10 @@
         <v>2</v>
       </c>
       <c r="E6" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F6" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -720,10 +865,10 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -734,13 +879,13 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -751,13 +896,13 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F9" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.25">
@@ -771,7 +916,7 @@
         <v>3</v>
       </c>
       <c r="F10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -785,10 +930,10 @@
         <v>3</v>
       </c>
       <c r="E11" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="F11" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
   </sheetData>
@@ -807,7 +952,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8353AB8B-5FB3-4C2E-B56B-5EAF5DE5DE00}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
@@ -833,10 +978,10 @@
         <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="F1" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="G1" t="s">
         <v>20</v>
@@ -866,10 +1011,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA036B15-B04C-4846-822B-68722C1605FF}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D3" sqref="D3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -905,22 +1050,276 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>30</v>
+        <v>54</v>
       </c>
       <c r="D2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E2">
         <v>2025</v>
       </c>
-      <c r="G2" t="s">
+      <c r="F2" t="s">
+        <v>57</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="C3" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" t="s">
+        <v>60</v>
+      </c>
+      <c r="E3">
+        <v>2025</v>
+      </c>
+      <c r="F3" t="s">
+        <v>61</v>
+      </c>
+      <c r="G3" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="C4" t="s">
+        <v>64</v>
+      </c>
+      <c r="D4" t="s">
+        <v>65</v>
+      </c>
+      <c r="E4">
+        <v>2025</v>
+      </c>
+      <c r="F4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="C5" t="s">
+        <v>69</v>
+      </c>
+      <c r="D5" t="s">
+        <v>65</v>
+      </c>
+      <c r="E5">
+        <v>2025</v>
+      </c>
+      <c r="F5" t="s">
+        <v>70</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="C6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D6" t="s">
+        <v>75</v>
+      </c>
+      <c r="E6">
+        <v>2025</v>
+      </c>
+      <c r="F6" t="s">
+        <v>74</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>78</v>
+      </c>
+      <c r="C7" t="s">
+        <v>77</v>
+      </c>
+      <c r="D7" t="s">
+        <v>79</v>
+      </c>
+      <c r="E7">
+        <v>2025</v>
+      </c>
+      <c r="F7" t="s">
+        <v>80</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C8" t="s">
+        <v>83</v>
+      </c>
+      <c r="D8" t="s">
         <v>55</v>
       </c>
+      <c r="E8">
+        <v>2025</v>
+      </c>
+      <c r="F8" t="s">
+        <v>84</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="C9" t="s">
+        <v>87</v>
+      </c>
+      <c r="D9" t="s">
+        <v>88</v>
+      </c>
+      <c r="E9">
+        <v>2025</v>
+      </c>
+      <c r="F9" t="s">
+        <v>90</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="C10" t="s">
+        <v>92</v>
+      </c>
+      <c r="D10" t="s">
+        <v>93</v>
+      </c>
+      <c r="E10">
+        <v>2025</v>
+      </c>
+      <c r="F10" t="s">
+        <v>104</v>
+      </c>
+      <c r="G10" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C11" t="s">
+        <v>95</v>
+      </c>
+      <c r="D11" t="s">
+        <v>88</v>
+      </c>
+      <c r="E11">
+        <v>2025</v>
+      </c>
+      <c r="F11" t="s">
+        <v>102</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="C12" t="s">
+        <v>97</v>
+      </c>
+      <c r="D12" t="s">
+        <v>98</v>
+      </c>
+      <c r="E12">
+        <v>2025</v>
+      </c>
+      <c r="F12" t="s">
+        <v>100</v>
+      </c>
+      <c r="G12" s="1" t="s">
+        <v>99</v>
+      </c>
     </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="G2" r:id="rId1" tooltip="Persistent link using digital object identifier" xr:uid="{8C4BE7AD-9B8A-4513-9DEA-B61B3E323081}"/>
+    <hyperlink ref="B3" r:id="rId2" display="https://www.nature.com/articles/s41597-025-05016-6" xr:uid="{C7AA57B3-1C06-4BB6-9862-8384601EF441}"/>
+    <hyperlink ref="B4" r:id="rId3" display="https://www.sciencedirect.com/science/article/pii/S0168169925001024" xr:uid="{859FBF44-1C93-452B-91CB-9BB83F81709D}"/>
+    <hyperlink ref="G4" r:id="rId4" tooltip="Persistent link using digital object identifier" xr:uid="{A18DB132-81A1-4820-B891-024F6151C082}"/>
+    <hyperlink ref="B5" r:id="rId5" display="https://www.sciencedirect.com/science/article/pii/S0168169925001437" xr:uid="{C1AAA1BF-B400-4A93-88F6-75B013DE419F}"/>
+    <hyperlink ref="G5" r:id="rId6" tooltip="Persistent link using digital object identifier" xr:uid="{4E055718-346D-4F36-811E-C7ECF7544DB3}"/>
+    <hyperlink ref="G6" r:id="rId7" tooltip="Persistent link using digital object identifier" xr:uid="{FB2409D0-4274-4D1F-8C28-0CEEA71A65C5}"/>
+    <hyperlink ref="B7" r:id="rId8" display="https://www.frontiersin.org/journals/plant-science/articles/10.3389/fpls.2025.1459126/full" xr:uid="{F6CC753E-1F27-484A-B201-1C2539849190}"/>
+    <hyperlink ref="G7" r:id="rId9" xr:uid="{23F20DB4-28CE-4076-83FA-E556423C383F}"/>
+    <hyperlink ref="B8" r:id="rId10" display="https://www.sciencedirect.com/science/article/pii/S0378429025000346" xr:uid="{7358009E-380C-48A7-838A-6F3986ED1656}"/>
+    <hyperlink ref="G8" r:id="rId11" tooltip="Persistent link using digital object identifier" xr:uid="{85066EAD-4FD2-4805-AF6F-B17ABB4DD6B9}"/>
+    <hyperlink ref="B9" r:id="rId12" display="https://acsess.onlinelibrary.wiley.com/doi/abs/10.1002/csc2.21449" xr:uid="{5FAEDD76-8286-42B6-8764-730ABA1F51AF}"/>
+    <hyperlink ref="G9" r:id="rId13" xr:uid="{4A2F33D6-9AF0-45A4-832C-38634A17FBDA}"/>
+    <hyperlink ref="B10" r:id="rId14" display="https://www.sciencedirect.com/science/article/pii/S1161030124003496" xr:uid="{C7736048-9942-49FA-89DB-889445CE9CAD}"/>
+    <hyperlink ref="B11" r:id="rId15" display="https://acsess.onlinelibrary.wiley.com/doi/abs/10.1002/csc2.21364" xr:uid="{98D8D144-03F4-4E91-954D-63328DF26A03}"/>
+    <hyperlink ref="B12" r:id="rId16" display="https://www.sciencedirect.com/science/article/pii/S0308521X24003032" xr:uid="{463418F6-191F-4AE4-B97E-C8C9A45547DC}"/>
+    <hyperlink ref="G12" r:id="rId17" tooltip="Persistent link using digital object identifier" xr:uid="{868AEF71-274B-4430-809C-63E8ACA5B3D4}"/>
+    <hyperlink ref="G11" r:id="rId18" xr:uid="{99FDAF04-1BE3-4283-8F42-9727449FC8B3}"/>
+    <hyperlink ref="G10" r:id="rId19" tooltip="Persistent link using digital object identifier" xr:uid="{0D6164FE-0D41-4542-95FF-835BF51F3784}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
chore: add pfp file names
</commit_message>
<xml_diff>
--- a/public/data/info.xlsx
+++ b/public/data/info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
-  <workbookPr defaultThemeVersion="202300"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\pedro\Ciampitti_Lab\ciampitti-lab.github.io\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\cisdeli\Purdue\CiampittiLab\ciampitti-lab.github.io\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0BAE9B87-34BF-4860-BDA9-2301C5EC7C3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A023D9-111B-41D2-8FC8-1063248C4BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
+    <workbookView xWindow="1125" yWindow="1125" windowWidth="28800" windowHeight="15345" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -29,8 +29,6 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -38,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="117" uniqueCount="105">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="115">
   <si>
     <t>role</t>
   </si>
@@ -130,9 +128,6 @@
     <t>Postdoc</t>
   </si>
   <si>
-    <t>Agronomist from Maringá, Brazil. Experienced in cropping systems, plant breeding, and seed tech.</t>
-  </si>
-  <si>
     <t>Agronomist from Arapongas, Brazil. Focused on crop modeling and digital ag, with experience in fatty acid analysis and on-farm data.</t>
   </si>
   <si>
@@ -353,13 +348,46 @@
   </si>
   <si>
     <t>https://www.sciencedirect.com/science/article/abs/pii/S1161030124003496</t>
+  </si>
+  <si>
+    <t>ignacio_ciampitti.jpg</t>
+  </si>
+  <si>
+    <t>gustavo_santiago.jpg</t>
+  </si>
+  <si>
+    <t>thatiane_pereira.jpg</t>
+  </si>
+  <si>
+    <t>german_mandrini.png</t>
+  </si>
+  <si>
+    <t>leonardo_bosche.jpg</t>
+  </si>
+  <si>
+    <t>franco_murinigo.jpg</t>
+  </si>
+  <si>
+    <t>natalia_volpato.jpg</t>
+  </si>
+  <si>
+    <t>federico_gomez.jpg</t>
+  </si>
+  <si>
+    <t>priscila_cano.jpg</t>
+  </si>
+  <si>
+    <t>pedro_cisdeli.png</t>
+  </si>
+  <si>
+    <t>Agronomist developing decision support models for precision nitrogen management in corn. Integrates crop physiology, sensing technologies, and statistics to improve productivity while reducing environmental impact.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -738,21 +766,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EB64B1-8415-484E-B4A1-A632CC3BB222}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="182.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="182.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -763,16 +791,16 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="E1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -780,16 +808,19 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
+        <v>48</v>
+      </c>
+      <c r="D2" t="s">
+        <v>104</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="F2" t="s">
         <v>49</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -799,14 +830,17 @@
       <c r="C3" t="s">
         <v>1</v>
       </c>
+      <c r="D3" t="s">
+        <v>113</v>
+      </c>
       <c r="E3" s="1" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -816,14 +850,17 @@
       <c r="C4" t="s">
         <v>2</v>
       </c>
+      <c r="D4" t="s">
+        <v>105</v>
+      </c>
       <c r="E4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F4" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -833,14 +870,17 @@
       <c r="C5" t="s">
         <v>2</v>
       </c>
+      <c r="D5" t="s">
+        <v>108</v>
+      </c>
       <c r="E5" s="1" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -850,14 +890,17 @@
       <c r="C6" t="s">
         <v>2</v>
       </c>
+      <c r="D6" t="s">
+        <v>110</v>
+      </c>
       <c r="E6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F6" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -867,11 +910,14 @@
       <c r="C7" t="s">
         <v>29</v>
       </c>
+      <c r="D7" t="s">
+        <v>111</v>
+      </c>
       <c r="F7" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -881,14 +927,17 @@
       <c r="C8" t="s">
         <v>29</v>
       </c>
+      <c r="D8" t="s">
+        <v>107</v>
+      </c>
       <c r="E8" s="1" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="F8" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
@@ -898,14 +947,17 @@
       <c r="C9" t="s">
         <v>29</v>
       </c>
+      <c r="D9" t="s">
+        <v>112</v>
+      </c>
       <c r="E9" s="1" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F9" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
@@ -915,11 +967,14 @@
       <c r="C10" t="s">
         <v>3</v>
       </c>
+      <c r="D10" t="s">
+        <v>109</v>
+      </c>
       <c r="F10" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
@@ -929,11 +984,14 @@
       <c r="C11" t="s">
         <v>3</v>
       </c>
+      <c r="D11" t="s">
+        <v>106</v>
+      </c>
       <c r="E11" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="F11" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
   </sheetData>
@@ -956,15 +1014,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -978,16 +1036,16 @@
         <v>19</v>
       </c>
       <c r="E1" t="s">
+        <v>50</v>
+      </c>
+      <c r="F1" t="s">
         <v>51</v>
-      </c>
-      <c r="F1" t="s">
-        <v>52</v>
       </c>
       <c r="G1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1013,16 +1071,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA036B15-B04C-4846-822B-68722C1605FF}">
   <dimension ref="A1:G12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F10" sqref="F10"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1045,257 +1103,257 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>52</v>
+      </c>
+      <c r="C2" t="s">
         <v>53</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>54</v>
-      </c>
-      <c r="D2" t="s">
-        <v>55</v>
       </c>
       <c r="E2">
         <v>2025</v>
       </c>
       <c r="F2" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="C3" t="s">
         <v>58</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>59</v>
-      </c>
-      <c r="D3" t="s">
-        <v>60</v>
       </c>
       <c r="E3">
         <v>2025</v>
       </c>
       <c r="F3" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" t="s">
         <v>61</v>
       </c>
-      <c r="G3" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C4" t="s">
         <v>63</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>64</v>
-      </c>
-      <c r="D4" t="s">
-        <v>65</v>
       </c>
       <c r="E4">
         <v>2025</v>
       </c>
       <c r="F4" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="C5" t="s">
         <v>68</v>
       </c>
-      <c r="C5" t="s">
-        <v>69</v>
-      </c>
       <c r="D5" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E5">
         <v>2025</v>
       </c>
       <c r="F5" t="s">
+        <v>69</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>70</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>71</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="C6" t="s">
         <v>72</v>
       </c>
-      <c r="C6" t="s">
-        <v>73</v>
-      </c>
       <c r="D6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="E6">
         <v>2025</v>
       </c>
       <c r="F6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>76</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="C7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D7" t="s">
         <v>78</v>
-      </c>
-      <c r="C7" t="s">
-        <v>77</v>
-      </c>
-      <c r="D7" t="s">
-        <v>79</v>
       </c>
       <c r="E7">
         <v>2025</v>
       </c>
       <c r="F7" t="s">
+        <v>79</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>80</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="C8" t="s">
         <v>82</v>
       </c>
-      <c r="C8" t="s">
-        <v>83</v>
-      </c>
       <c r="D8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="E8">
         <v>2025</v>
       </c>
       <c r="F8" t="s">
+        <v>83</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>84</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>85</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="C9" t="s">
         <v>86</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>87</v>
-      </c>
-      <c r="D9" t="s">
-        <v>88</v>
       </c>
       <c r="E9">
         <v>2025</v>
       </c>
       <c r="F9" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>89</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="C10" t="s">
         <v>91</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>92</v>
-      </c>
-      <c r="D10" t="s">
-        <v>93</v>
       </c>
       <c r="E10">
         <v>2025</v>
       </c>
       <c r="F10" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>103</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="C11" t="s">
         <v>94</v>
       </c>
-      <c r="C11" t="s">
-        <v>95</v>
-      </c>
       <c r="D11" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="E11">
         <v>2025</v>
       </c>
       <c r="F11" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="C12" t="s">
         <v>96</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>97</v>
-      </c>
-      <c r="D12" t="s">
-        <v>98</v>
       </c>
       <c r="E12">
         <v>2025</v>
       </c>
       <c r="F12" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: adjust pfp file name
</commit_message>
<xml_diff>
--- a/public/data/info.xlsx
+++ b/public/data/info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\cisdeli\Purdue\CiampittiLab\ciampitti-lab.github.io\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\pedro\Ciampitti_Lab\ciampitti-lab.github.io\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A023D9-111B-41D2-8FC8-1063248C4BB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CBCEF4-FEB6-45CD-BB68-5BBA2717F18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1125" yWindow="1125" windowWidth="28800" windowHeight="15345" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -377,17 +377,17 @@
     <t>priscila_cano.jpg</t>
   </si>
   <si>
-    <t>pedro_cisdeli.png</t>
-  </si>
-  <si>
     <t>Agronomist developing decision support models for precision nitrogen management in corn. Integrates crop physiology, sensing technologies, and statistics to improve productivity while reducing environmental impact.</t>
+  </si>
+  <si>
+    <t>pedro_cisdeli.jpg</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,10 +425,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -766,21 +765,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EB64B1-8415-484E-B4A1-A632CC3BB222}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="182.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="182.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -800,7 +799,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -820,7 +819,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -831,7 +830,7 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="E3" s="1" t="s">
         <v>41</v>
@@ -840,7 +839,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -860,7 +859,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -877,10 +876,10 @@
         <v>43</v>
       </c>
       <c r="F5" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -900,7 +899,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -917,7 +916,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -937,7 +936,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -957,7 +956,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -974,7 +973,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1014,15 +1013,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1045,7 +1044,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1075,12 +1074,12 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1103,7 +1102,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1126,7 +1125,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1149,7 +1148,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1172,7 +1171,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1195,11 +1194,11 @@
         <v>70</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" t="s">
         <v>71</v>
       </c>
       <c r="C6" t="s">
@@ -1218,7 +1217,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1241,7 +1240,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1264,7 +1263,7 @@
         <v>84</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1287,7 +1286,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1310,7 +1309,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1333,7 +1332,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
chore: correct research interests - priscila
</commit_message>
<xml_diff>
--- a/public/data/info.xlsx
+++ b/public/data/info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\pedro\Ciampitti_Lab\ciampitti-lab.github.io\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\cisdeli\Purdue\CiampittiLab\ciampitti-lab.github.io\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{85CBCEF4-FEB6-45CD-BB68-5BBA2717F18E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E960F5-1099-449A-BB53-A3CCBF65771E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
+    <workbookView xWindow="25605" yWindow="900" windowWidth="12615" windowHeight="19785" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -137,9 +137,6 @@
     <t>ML engineer bridging computer science and agronomy. Focused on computer vision, 3D reconstruction, data analysis and precision ag.</t>
   </si>
   <si>
-    <t>Researches sustainable ag systems using modeling, remote sensing, and digital tools to understand impacts from field to global scale.</t>
-  </si>
-  <si>
     <t>Focuses on crop modeling and data analysis. Background in agronomy with research on yield gaps, nutrient dynamics, and malting barley quality.</t>
   </si>
   <si>
@@ -381,13 +378,16 @@
   </si>
   <si>
     <t>pedro_cisdeli.jpg</t>
+  </si>
+  <si>
+    <t>Combining expertise in agronomy, remote sensing &amp; geographic information systems, and economics. Current research efforts are directed toward the sustainable intensification of agricultural systems and digital agriculture.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -425,9 +425,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -765,21 +768,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EB64B1-8415-484E-B4A1-A632CC3BB222}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="182.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.75" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="182.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -790,16 +793,16 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="E1" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -807,19 +810,19 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
+        <v>47</v>
+      </c>
+      <c r="D2" t="s">
+        <v>103</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" t="s">
         <v>48</v>
       </c>
-      <c r="D2" t="s">
-        <v>104</v>
-      </c>
-      <c r="E2" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F2" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -830,16 +833,16 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F3" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -850,16 +853,16 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="E4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="F4" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -870,16 +873,16 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="F5" t="s">
-        <v>113</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -890,16 +893,16 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="E6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="F6" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -910,13 +913,13 @@
         <v>29</v>
       </c>
       <c r="D7" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="F7" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -927,16 +930,16 @@
         <v>29</v>
       </c>
       <c r="D8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="F8" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.5">
       <c r="A9">
         <v>8</v>
       </c>
@@ -947,16 +950,16 @@
         <v>29</v>
       </c>
       <c r="D9" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="F9" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>45</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
@@ -967,13 +970,13 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F10" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
@@ -984,13 +987,13 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="E11" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="F11" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
   </sheetData>
@@ -1013,15 +1016,15 @@
       <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1035,16 +1038,16 @@
         <v>19</v>
       </c>
       <c r="E1" t="s">
+        <v>49</v>
+      </c>
+      <c r="F1" t="s">
         <v>50</v>
-      </c>
-      <c r="F1" t="s">
-        <v>51</v>
       </c>
       <c r="G1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1074,12 +1077,12 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1102,257 +1105,257 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
         <v>52</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>53</v>
-      </c>
-      <c r="D2" t="s">
-        <v>54</v>
       </c>
       <c r="E2">
         <v>2025</v>
       </c>
       <c r="F2" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="C3" t="s">
         <v>57</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>58</v>
-      </c>
-      <c r="D3" t="s">
-        <v>59</v>
       </c>
       <c r="E3">
         <v>2025</v>
       </c>
       <c r="F3" t="s">
+        <v>59</v>
+      </c>
+      <c r="G3" t="s">
         <v>60</v>
       </c>
-      <c r="G3" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="C4" t="s">
         <v>62</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>63</v>
-      </c>
-      <c r="D4" t="s">
-        <v>64</v>
       </c>
       <c r="E4">
         <v>2025</v>
       </c>
       <c r="F4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" t="s">
         <v>67</v>
       </c>
-      <c r="C5" t="s">
-        <v>68</v>
-      </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E5">
         <v>2025</v>
       </c>
       <c r="F5" t="s">
+        <v>68</v>
+      </c>
+      <c r="G5" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="G5" s="1" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C6" t="s">
         <v>71</v>
       </c>
-      <c r="C6" t="s">
-        <v>72</v>
-      </c>
       <c r="D6" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="E6">
         <v>2025</v>
       </c>
       <c r="F6" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="C7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D7" t="s">
         <v>77</v>
-      </c>
-      <c r="C7" t="s">
-        <v>76</v>
-      </c>
-      <c r="D7" t="s">
-        <v>78</v>
       </c>
       <c r="E7">
         <v>2025</v>
       </c>
       <c r="F7" t="s">
+        <v>78</v>
+      </c>
+      <c r="G7" s="1" t="s">
         <v>79</v>
       </c>
-      <c r="G7" s="1" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="C8" t="s">
         <v>81</v>
       </c>
-      <c r="C8" t="s">
-        <v>82</v>
-      </c>
       <c r="D8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="E8">
         <v>2025</v>
       </c>
       <c r="F8" t="s">
+        <v>82</v>
+      </c>
+      <c r="G8" s="1" t="s">
         <v>83</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="C9" t="s">
         <v>85</v>
       </c>
-      <c r="C9" t="s">
+      <c r="D9" t="s">
         <v>86</v>
-      </c>
-      <c r="D9" t="s">
-        <v>87</v>
       </c>
       <c r="E9">
         <v>2025</v>
       </c>
       <c r="F9" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="C10" t="s">
         <v>90</v>
       </c>
-      <c r="C10" t="s">
+      <c r="D10" t="s">
         <v>91</v>
-      </c>
-      <c r="D10" t="s">
-        <v>92</v>
       </c>
       <c r="E10">
         <v>2025</v>
       </c>
       <c r="F10" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>102</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C11" t="s">
         <v>93</v>
       </c>
-      <c r="C11" t="s">
-        <v>94</v>
-      </c>
       <c r="D11" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="E11">
         <v>2025</v>
       </c>
       <c r="F11" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="C12" t="s">
         <v>95</v>
       </c>
-      <c r="C12" t="s">
+      <c r="D12" t="s">
         <v>96</v>
-      </c>
-      <c r="D12" t="s">
-        <v>97</v>
       </c>
       <c r="E12">
         <v>2025</v>
       </c>
       <c r="F12" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat: blog posts; needs fine tunning
</commit_message>
<xml_diff>
--- a/public/data/info.xlsx
+++ b/public/data/info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\cisdeli\Purdue\CiampittiLab\ciampitti-lab.github.io\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3E960F5-1099-449A-BB53-A3CCBF65771E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79844157-B55F-489B-9516-44DB524ADBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="25605" yWindow="900" windowWidth="12615" windowHeight="19785" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
+    <workbookView xWindow="14445" yWindow="900" windowWidth="14160" windowHeight="16185" activeTab="1" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="127" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="117">
   <si>
     <t>role</t>
   </si>
@@ -381,6 +381,12 @@
   </si>
   <si>
     <t>Combining expertise in agronomy, remote sensing &amp; geographic information systems, and economics. Current research efforts are directed toward the sustainable intensification of agricultural systems and digital agriculture.</t>
+  </si>
+  <si>
+    <t>hello_world.md</t>
+  </si>
+  <si>
+    <t>hello_word.png</t>
   </si>
 </sst>
 </file>
@@ -768,7 +774,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EB64B1-8415-484E-B4A1-A632CC3BB222}">
   <dimension ref="A1:F11"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
@@ -1012,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8353AB8B-5FB3-4C2E-B56B-5EAF5DE5DE00}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1062,6 +1068,12 @@
       </c>
       <c r="E2" t="s">
         <v>21</v>
+      </c>
+      <c r="F2" t="s">
+        <v>115</v>
+      </c>
+      <c r="G2" t="s">
+        <v>116</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: first post; should add the GH org to it later
</commit_message>
<xml_diff>
--- a/public/data/info.xlsx
+++ b/public/data/info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\cisdeli\Purdue\CiampittiLab\ciampitti-lab.github.io\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\pedro\Ciampitti_Lab\ciampitti-lab.github.io\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79844157-B55F-489B-9516-44DB524ADBD6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36CB129C-5258-40F8-BC4D-C1D80C5B47ED}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14445" yWindow="900" windowWidth="14160" windowHeight="16185" activeTab="1" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="118">
   <si>
     <t>role</t>
   </si>
@@ -101,12 +101,6 @@
     <t>img_file_name</t>
   </si>
   <si>
-    <t>Test</t>
-  </si>
-  <si>
-    <t>This is a test</t>
-  </si>
-  <si>
     <t>May 08, 2025</t>
   </si>
   <si>
@@ -386,14 +380,23 @@
     <t>hello_world.md</t>
   </si>
   <si>
-    <t>hello_word.png</t>
+    <t>hello_world.png</t>
+  </si>
+  <si>
+    <t>We’re thrilled to join Purdue University and to unveil our redesigned online home.</t>
+  </si>
+  <si>
+    <t>A New Chapter: Ciampitti Lab Moves to Purdue &amp; Launches a Fresh Website</t>
+  </si>
+  <si>
+    <t>General</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -778,17 +781,17 @@
       <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="182.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="182.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -799,16 +802,16 @@
         <v>0</v>
       </c>
       <c r="D1" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="E1" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="F1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -816,19 +819,19 @@
         <v>15</v>
       </c>
       <c r="C2" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D2" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -839,16 +842,16 @@
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F3" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -859,16 +862,16 @@
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="E4" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F4" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -879,16 +882,16 @@
         <v>2</v>
       </c>
       <c r="D5" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="F5" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="6" spans="1:6">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -899,16 +902,16 @@
         <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E6" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="7" spans="1:6">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -916,16 +919,16 @@
         <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D7" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="F7" t="s">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:6">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -933,19 +936,19 @@
         <v>12</v>
       </c>
       <c r="C8" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D8" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F8" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="28.5">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -953,19 +956,19 @@
         <v>10</v>
       </c>
       <c r="C9" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="D9" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F9" s="2" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -976,13 +979,13 @@
         <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="F10" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="11" spans="1:6">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -993,13 +996,13 @@
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="E11" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
     </row>
   </sheetData>
@@ -1019,18 +1022,18 @@
   <dimension ref="A1:G2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G3" sqref="G3"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1044,36 +1047,36 @@
         <v>19</v>
       </c>
       <c r="E1" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="F1" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>116</v>
+      </c>
+      <c r="C2" t="s">
+        <v>115</v>
+      </c>
+      <c r="D2" t="s">
         <v>21</v>
       </c>
-      <c r="C2" t="s">
-        <v>22</v>
-      </c>
-      <c r="D2" t="s">
-        <v>23</v>
-      </c>
       <c r="E2" t="s">
-        <v>21</v>
+        <v>117</v>
       </c>
       <c r="F2" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="G2" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
   </sheetData>
@@ -1089,12 +1092,12 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1102,272 +1105,272 @@
         <v>17</v>
       </c>
       <c r="C1" t="s">
+        <v>22</v>
+      </c>
+      <c r="D1" t="s">
+        <v>23</v>
+      </c>
+      <c r="E1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F1" t="s">
         <v>24</v>
       </c>
-      <c r="D1" t="s">
+      <c r="G1" t="s">
         <v>25</v>
       </c>
-      <c r="E1" t="s">
-        <v>28</v>
-      </c>
-      <c r="F1" t="s">
-        <v>26</v>
-      </c>
-      <c r="G1" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>49</v>
+      </c>
+      <c r="C2" t="s">
+        <v>50</v>
+      </c>
+      <c r="D2" t="s">
         <v>51</v>
-      </c>
-      <c r="C2" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" t="s">
-        <v>53</v>
       </c>
       <c r="E2">
         <v>2025</v>
       </c>
       <c r="F2" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" s="1" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" t="s">
+        <v>55</v>
+      </c>
+      <c r="D3" t="s">
         <v>56</v>
-      </c>
-      <c r="C3" t="s">
-        <v>57</v>
-      </c>
-      <c r="D3" t="s">
-        <v>58</v>
       </c>
       <c r="E3">
         <v>2025</v>
       </c>
       <c r="F3" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="G3" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C4" t="s">
+        <v>60</v>
+      </c>
+      <c r="D4" t="s">
         <v>61</v>
-      </c>
-      <c r="C4" t="s">
-        <v>62</v>
-      </c>
-      <c r="D4" t="s">
-        <v>63</v>
       </c>
       <c r="E4">
         <v>2025</v>
       </c>
       <c r="F4" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C5" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="E5">
         <v>2025</v>
       </c>
       <c r="F5" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C6" t="s">
+        <v>69</v>
+      </c>
+      <c r="D6" t="s">
         <v>71</v>
-      </c>
-      <c r="D6" t="s">
-        <v>73</v>
       </c>
       <c r="E6">
         <v>2025</v>
       </c>
       <c r="F6" t="s">
+        <v>70</v>
+      </c>
+      <c r="G6" s="1" t="s">
         <v>72</v>
       </c>
-      <c r="G6" s="1" t="s">
-        <v>74</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7">
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="C7" t="s">
+        <v>73</v>
+      </c>
+      <c r="D7" t="s">
         <v>75</v>
-      </c>
-      <c r="D7" t="s">
-        <v>77</v>
       </c>
       <c r="E7">
         <v>2025</v>
       </c>
       <c r="F7" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="C8" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="E8">
         <v>2025</v>
       </c>
       <c r="F8" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="C9" t="s">
+        <v>83</v>
+      </c>
+      <c r="D9" t="s">
         <v>84</v>
-      </c>
-      <c r="C9" t="s">
-        <v>85</v>
-      </c>
-      <c r="D9" t="s">
-        <v>86</v>
       </c>
       <c r="E9">
         <v>2025</v>
       </c>
       <c r="F9" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>87</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C10" t="s">
+        <v>88</v>
+      </c>
+      <c r="D10" t="s">
         <v>89</v>
-      </c>
-      <c r="C10" t="s">
-        <v>90</v>
-      </c>
-      <c r="D10" t="s">
-        <v>91</v>
       </c>
       <c r="E10">
         <v>2025</v>
       </c>
       <c r="F10" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>101</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C11" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D11" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E11">
         <v>2025</v>
       </c>
       <c r="F11" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="C12" t="s">
+        <v>93</v>
+      </c>
+      <c r="D12" t="s">
         <v>94</v>
-      </c>
-      <c r="C12" t="s">
-        <v>95</v>
-      </c>
-      <c r="D12" t="s">
-        <v>96</v>
       </c>
       <c r="E12">
         <v>2025</v>
       </c>
       <c r="F12" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
chore: add Francisco to the database
</commit_message>
<xml_diff>
--- a/public/data/info.xlsx
+++ b/public/data/info.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\pedro\Ciampitti_Lab\ciampitti-lab.github.io\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{224ADFE9-38E5-4379-AB0E-489C7BA0C9D4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE94DFC-16B5-4CAD-AC76-A26ADFBC5242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="122">
   <si>
     <t>role</t>
   </si>
@@ -390,6 +390,18 @@
   </si>
   <si>
     <t>Agronomist researching sustainable corn-soybean systems, using digital tools to assess how crop rotation, cover crops, and nitrogen management impact soil health, environmental resilience, and overall farm productivity and profitability.</t>
+  </si>
+  <si>
+    <t>francisco_palmero.jpg</t>
+  </si>
+  <si>
+    <t>Francisco Palmero</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/francisco-palmero-6b8826170/</t>
+  </si>
+  <si>
+    <t>Focuses on applied statistics for agriculture-related problems, with emphasis on nitrogen management and corn physiology. Background in the role of legume crops in soil nitrogen budgets within agricultural systems.</t>
   </si>
 </sst>
 </file>
@@ -775,15 +787,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EB64B1-8415-484E-B4A1-A632CC3BB222}">
-  <dimension ref="A1:F11"/>
+  <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="F8" sqref="F8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="2.7109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
@@ -933,56 +945,59 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>12</v>
+        <v>119</v>
       </c>
       <c r="C8" t="s">
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>102</v>
+        <v>118</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>40</v>
+        <v>120</v>
       </c>
       <c r="F8" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>10</v>
+        <v>12</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F9" s="2" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.25">
+        <v>40</v>
+      </c>
+      <c r="F9" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>14</v>
+        <v>10</v>
       </c>
       <c r="C10" t="s">
-        <v>3</v>
+        <v>26</v>
       </c>
       <c r="D10" t="s">
-        <v>104</v>
-      </c>
-      <c r="F10" t="s">
-        <v>32</v>
+        <v>107</v>
+      </c>
+      <c r="E10" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="F10" s="2" t="s">
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -990,18 +1005,35 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11" t="s">
+        <v>104</v>
+      </c>
+      <c r="F11" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>13</v>
+      </c>
+      <c r="C12" t="s">
+        <v>3</v>
+      </c>
+      <c r="D12" t="s">
         <v>101</v>
       </c>
-      <c r="E11" t="s">
+      <c r="E12" t="s">
         <v>42</v>
       </c>
-      <c r="F11" t="s">
+      <c r="F12" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1010,8 +1042,7 @@
     <hyperlink ref="E3" r:id="rId1" xr:uid="{AAA55F43-9F3C-40DB-9B47-46AAC432FF09}"/>
     <hyperlink ref="E2" r:id="rId2" xr:uid="{A94255E5-8ECE-483E-BE8F-EE9B37DAE260}"/>
     <hyperlink ref="E5" r:id="rId3" xr:uid="{F9808E56-71B8-4EF9-927B-9D68DAE7673D}"/>
-    <hyperlink ref="E8" r:id="rId4" xr:uid="{F482682B-7EA6-4322-99D1-4928E3914F09}"/>
-    <hyperlink ref="E9" r:id="rId5" xr:uid="{12A704E9-6647-4B36-9BA4-2702987CAED0}"/>
+    <hyperlink ref="E9" r:id="rId4" xr:uid="{2A6658AF-7FC0-4FB5-9A94-14DD4D416741}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
chore: add caetano and diogo
</commit_message>
<xml_diff>
--- a/public/data/info.xlsx
+++ b/public/data/info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28730"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\pedro\Ciampitti_Lab\ciampitti-lab.github.io\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\cisdeli\Purdue\CiampittiLab\ciampitti-lab.github.io\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1CE94DFC-16B5-4CAD-AC76-A26ADFBC5242}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6EC15B88-6FE2-481D-B387-4E282561B467}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="134" uniqueCount="122">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="144" uniqueCount="130">
   <si>
     <t>role</t>
   </si>
@@ -402,13 +402,37 @@
   </si>
   <si>
     <t>Focuses on applied statistics for agriculture-related problems, with emphasis on nitrogen management and corn physiology. Background in the role of legume crops in soil nitrogen budgets within agricultural systems.</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/diogo-verzegnazzi-555418239/</t>
+  </si>
+  <si>
+    <t>Diogo Verzegnazzi</t>
+  </si>
+  <si>
+    <t>diogo_verzegnazzi.jpg</t>
+  </si>
+  <si>
+    <t>Caetano Rocha</t>
+  </si>
+  <si>
+    <t>caetano_rocha.jpg</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/caetano-rocha-9087b0319/</t>
+  </si>
+  <si>
+    <t>Agronomy undergraduate from University of Santa Maria with experience in field crops. Supports field operations through crop monitoring, data collection, and hands-on agricultural practices across research sites.</t>
+  </si>
+  <si>
+    <t>Agronomy undergraduate from University of Santa Maria with experience in field crops and soil science. Supports field operations through crop monitoring, data collection, and hands-on agricultural practices across research sites.</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -787,23 +811,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EB64B1-8415-484E-B4A1-A632CC3BB222}">
-  <dimension ref="A1:F12"/>
+  <dimension ref="A1:F14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="182.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="182.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -823,7 +847,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -843,7 +867,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -863,7 +887,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -883,7 +907,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -903,7 +927,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -923,7 +947,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -940,7 +964,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -960,7 +984,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -980,7 +1004,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1000,40 +1024,80 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>14</v>
+        <v>125</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>104</v>
+        <v>126</v>
+      </c>
+      <c r="E11" t="s">
+        <v>127</v>
       </c>
       <c r="F11" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>123</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
       </c>
       <c r="D12" t="s">
+        <v>124</v>
+      </c>
+      <c r="E12" t="s">
+        <v>122</v>
+      </c>
+      <c r="F12" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="13" spans="1:6">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>14</v>
+      </c>
+      <c r="C13" t="s">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>104</v>
+      </c>
+      <c r="F13" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="14" spans="1:6" ht="15">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" t="s">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
+        <v>3</v>
+      </c>
+      <c r="D14" t="s">
         <v>101</v>
       </c>
-      <c r="E12" t="s">
+      <c r="E14" t="s">
         <v>42</v>
       </c>
-      <c r="F12" t="s">
+      <c r="F14" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1056,15 +1120,15 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.8984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1087,7 +1151,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1123,12 +1187,12 @@
       <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1151,7 +1215,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1174,7 +1238,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1197,7 +1261,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1220,7 +1284,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1243,7 +1307,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1266,7 +1330,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1289,7 +1353,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1312,7 +1376,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1335,7 +1399,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1358,7 +1422,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1381,7 +1445,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>

</xml_diff>

<commit_message>
chore: add roberto linkedin
</commit_message>
<xml_diff>
--- a/public/data/info.xlsx
+++ b/public/data/info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\pedro\Ciampitti_Lab\ciampitti-lab.github.io\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\cisdeli\Purdue\CiampittiLab\ciampitti-lab.github.io\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02C9278-9448-434D-A41A-AED5EFB4C185}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D99ABA72-2517-4BEB-A412-1FF2AC08EFBF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="138">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="154" uniqueCount="139">
   <si>
     <t>role</t>
   </si>
@@ -450,13 +450,16 @@
   </si>
   <si>
     <t>https://doi.org/10.1007/s11119-025-10257-x</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/roberto-carlos-romero-palomeque-831917252?utm_source=share&amp;utm_campaign=share_via&amp;utm_content=profile&amp;utm_medium=ios_app</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -837,21 +840,21 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EB64B1-8415-484E-B4A1-A632CC3BB222}">
   <dimension ref="A1:F15"/>
   <sheetViews>
-    <sheetView topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="F19" sqref="F19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="182.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="182.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -871,7 +874,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -891,7 +894,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -911,7 +914,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -931,7 +934,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -951,7 +954,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -971,7 +974,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -988,7 +991,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1008,7 +1011,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1028,7 +1031,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1048,7 +1051,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1068,7 +1071,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1088,7 +1091,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1105,7 +1108,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1118,11 +1121,14 @@
       <c r="D14" t="s">
         <v>131</v>
       </c>
+      <c r="E14" s="1" t="s">
+        <v>138</v>
+      </c>
       <c r="F14" t="s">
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1148,6 +1154,7 @@
     <hyperlink ref="E2" r:id="rId2" xr:uid="{A94255E5-8ECE-483E-BE8F-EE9B37DAE260}"/>
     <hyperlink ref="E5" r:id="rId3" xr:uid="{F9808E56-71B8-4EF9-927B-9D68DAE7673D}"/>
     <hyperlink ref="E9" r:id="rId4" xr:uid="{2A6658AF-7FC0-4FB5-9A94-14DD4D416741}"/>
+    <hyperlink ref="E14" r:id="rId5" xr:uid="{D4CFB1C7-1AE1-491B-850A-B6BFAE8BB6A7}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1161,15 +1168,15 @@
       <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.8984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1192,7 +1199,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1224,16 +1231,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA036B15-B04C-4846-822B-68722C1605FF}">
   <dimension ref="A1:G13"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1256,7 +1263,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1279,7 +1286,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1302,7 +1309,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1325,7 +1332,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1348,7 +1355,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1371,7 +1378,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1394,7 +1401,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1417,7 +1424,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1440,7 +1447,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1463,7 +1470,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1486,7 +1493,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1509,7 +1516,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>

</xml_diff>

<commit_message>
chore: add slug to news data
</commit_message>
<xml_diff>
--- a/public/data/info.xlsx
+++ b/public/data/info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\cisdeli\Purdue\CiampittiLab\ciampitti-lab.github.io\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82DC5BBE-EF8D-4771-9092-729E2F0C8E21}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F612ED91-E8CB-4D04-8578-ED9F831D9385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="2" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="143">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="145">
   <si>
     <t>role</t>
   </si>
@@ -465,6 +465,12 @@
   </si>
   <si>
     <t>CVPR Workshop Proceedings</t>
+  </si>
+  <si>
+    <t>slug</t>
+  </si>
+  <si>
+    <t>ciampitti-lab-new-chapter</t>
   </si>
 </sst>
 </file>
@@ -1174,10 +1180,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8353AB8B-5FB3-4C2E-B56B-5EAF5DE5DE00}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1188,7 +1194,7 @@
     <col min="6" max="6" width="13.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1196,22 +1202,25 @@
         <v>17</v>
       </c>
       <c r="C1" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" t="s">
         <v>18</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>19</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>45</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1219,18 +1228,21 @@
         <v>114</v>
       </c>
       <c r="C2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D2" t="s">
         <v>113</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>116</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>115</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>111</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>112</v>
       </c>
     </row>
@@ -1243,7 +1255,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BA036B15-B04C-4846-822B-68722C1605FF}">
   <dimension ref="A1:G14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
chore: avp part 1 post
</commit_message>
<xml_diff>
--- a/public/data/info.xlsx
+++ b/public/data/info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24332"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\cisdeli\Purdue\CiampittiLab\ciampitti-lab.github.io\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\pedro\Ciampitti_Lab\ciampitti-lab.github.io\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F612ED91-E8CB-4D04-8578-ED9F831D9385}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883714F5-9222-426C-8F19-C34A9AC40C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
+    <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="145">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="151">
   <si>
     <t>role</t>
   </si>
@@ -471,13 +471,31 @@
   </si>
   <si>
     <t>ciampitti-lab-new-chapter</t>
+  </si>
+  <si>
+    <t>building-for-apple-vision-pro-1</t>
+  </si>
+  <si>
+    <t>Short series documenting Pedro Cisdeli's hands‑on journey building ag‑tech tools for Apple Vision Pro</t>
+  </si>
+  <si>
+    <t>June 27, 2025</t>
+  </si>
+  <si>
+    <t>developing_for_avp_part_1.md</t>
+  </si>
+  <si>
+    <t>developing_for_avp_part_1.png</t>
+  </si>
+  <si>
+    <t>Building for Apple Vision Pro: Part 1</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -862,17 +880,17 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="182.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="182.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -892,7 +910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -912,7 +930,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -932,7 +950,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -952,7 +970,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:6">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -972,7 +990,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:6">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -992,7 +1010,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1009,7 +1027,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1029,7 +1047,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:6">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1049,7 +1067,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1069,7 +1087,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:6">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1089,7 +1107,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:6">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1109,7 +1127,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:6">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1126,7 +1144,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1146,7 +1164,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:6">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1180,21 +1198,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8353AB8B-5FB3-4C2E-B56B-5EAF5DE5DE00}">
-  <dimension ref="A1:H2"/>
+  <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1220,7 +1238,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1244,6 +1262,32 @@
       </c>
       <c r="H2" t="s">
         <v>112</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>150</v>
+      </c>
+      <c r="C3" t="s">
+        <v>145</v>
+      </c>
+      <c r="D3" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" t="s">
+        <v>147</v>
+      </c>
+      <c r="F3" t="s">
+        <v>115</v>
+      </c>
+      <c r="G3" t="s">
+        <v>148</v>
+      </c>
+      <c r="H3" t="s">
+        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1259,12 +1303,12 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1287,7 +1331,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1310,7 +1354,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1333,7 +1377,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1356,7 +1400,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:7">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1379,7 +1423,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:7">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1402,7 +1446,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:7">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1425,7 +1469,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:7">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1448,7 +1492,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:7">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1471,7 +1515,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:7">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1494,7 +1538,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:7">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1517,7 +1561,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:7">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1540,7 +1584,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:7">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1563,7 +1607,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:7">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
minor changes to chars
</commit_message>
<xml_diff>
--- a/public/data/info.xlsx
+++ b/public/data/info.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28827"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu-20.04\home\pedro\Ciampitti_Lab\ciampitti-lab.github.io\public\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\cisdeli\Purdue\CiampittiLab\ciampitti-lab.github.io\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{883714F5-9222-426C-8F19-C34A9AC40C92}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CB619B-AAA1-4531-BDBC-2B3F0E65C99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1080" yWindow="1080" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -476,9 +476,6 @@
     <t>building-for-apple-vision-pro-1</t>
   </si>
   <si>
-    <t>Short series documenting Pedro Cisdeli's hands‑on journey building ag‑tech tools for Apple Vision Pro</t>
-  </si>
-  <si>
     <t>June 27, 2025</t>
   </si>
   <si>
@@ -489,13 +486,16 @@
   </si>
   <si>
     <t>Building for Apple Vision Pro: Part 1</t>
+  </si>
+  <si>
+    <t>Short series documenting Pedro Cisdeli's hands-on journey building ag-tech tools for Apple Vision Pro</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="2">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -880,17 +880,17 @@
       <selection activeCell="E19" sqref="E19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.5703125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.42578125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="182.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.59765625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.8984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="182.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" ht="15">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -910,7 +910,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:6" ht="15">
       <c r="A2">
         <v>1</v>
       </c>
@@ -930,7 +930,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:6" ht="15">
       <c r="A3">
         <v>2</v>
       </c>
@@ -950,7 +950,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" ht="15">
       <c r="A4">
         <v>3</v>
       </c>
@@ -970,7 +970,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" ht="15">
       <c r="A5">
         <v>4</v>
       </c>
@@ -990,7 +990,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" ht="15">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1010,7 +1010,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" ht="15">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" ht="15">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1047,7 +1047,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" ht="15">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1067,7 +1067,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" ht="30">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1087,7 +1087,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" ht="15">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1107,7 +1107,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" ht="15">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1127,7 +1127,7 @@
         <v>128</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1144,7 +1144,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" ht="15">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1164,7 +1164,7 @@
         <v>132</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" ht="15">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1201,18 +1201,18 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
-    <col min="3" max="3" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.8984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.3984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1238,7 +1238,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1264,30 +1264,30 @@
         <v>112</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C3" t="s">
         <v>145</v>
       </c>
       <c r="D3" t="s">
+        <v>150</v>
+      </c>
+      <c r="E3" t="s">
         <v>146</v>
-      </c>
-      <c r="E3" t="s">
-        <v>147</v>
       </c>
       <c r="F3" t="s">
         <v>115</v>
       </c>
       <c r="G3" t="s">
+        <v>147</v>
+      </c>
+      <c r="H3" t="s">
         <v>148</v>
-      </c>
-      <c r="H3" t="s">
-        <v>149</v>
       </c>
     </row>
   </sheetData>
@@ -1303,12 +1303,12 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="13.8"/>
   <cols>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -1331,7 +1331,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1354,7 +1354,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1377,7 +1377,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1400,7 +1400,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1423,7 +1423,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1446,7 +1446,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1469,7 +1469,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1492,7 +1492,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1515,7 +1515,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1538,7 +1538,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1561,7 +1561,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1584,7 +1584,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1607,7 +1607,7 @@
         <v>137</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7">
       <c r="A14">
         <v>13</v>
       </c>

</xml_diff>

<commit_message>
chore: add jorge to team members
</commit_message>
<xml_diff>
--- a/public/data/info.xlsx
+++ b/public/data/info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\cisdeli\Purdue\CiampittiLab\ciampitti-lab.github.io\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{44CB619B-AAA1-4531-BDBC-2B3F0E65C99C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9ACD510-ACB0-48AC-AFAE-1AFE2EDF1D3A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" activeTab="1" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
+    <workbookView xWindow="12" yWindow="12" windowWidth="23016" windowHeight="13656" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -31,12 +31,15 @@
         <xcalcf:feature name="microsoft.com:LET_WF"/>
       </xcalcf:calcFeatures>
     </ext>
+    <ext xmlns:xlwcv="http://schemas.microsoft.com/office/spreadsheetml/2024/workbookCompatibilityVersion" uri="{D14903EA-33C4-47F7-8F05-3474C54BE107}">
+      <xlwcv:version setVersion="1"/>
+    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="167" uniqueCount="151">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="156">
   <si>
     <t>role</t>
   </si>
@@ -489,6 +492,21 @@
   </si>
   <si>
     <t>Short series documenting Pedro Cisdeli's hands-on journey building ag-tech tools for Apple Vision Pro</t>
+  </si>
+  <si>
+    <t>Juan Fiore</t>
+  </si>
+  <si>
+    <t>jorge_jola.jpg</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/jjola-unal/</t>
+  </si>
+  <si>
+    <t>Jorge Jola</t>
+  </si>
+  <si>
+    <t>Undergraduate student in Agronomic Engineering at the National University of Colombia, with experience in agronomic data analysis. Skilled in statistics, Web applications, and the application of machine learning in agriculture.</t>
   </si>
 </sst>
 </file>
@@ -874,23 +892,23 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EB64B1-8415-484E-B4A1-A632CC3BB222}">
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="182.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="182.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15">
+    <row r="1" spans="1:6">
       <c r="A1" t="s">
         <v>16</v>
       </c>
@@ -910,7 +928,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="2" spans="1:6" ht="15">
+    <row r="2" spans="1:6">
       <c r="A2">
         <v>1</v>
       </c>
@@ -930,7 +948,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="3" spans="1:6" ht="15">
+    <row r="3" spans="1:6">
       <c r="A3">
         <v>2</v>
       </c>
@@ -950,7 +968,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:6" ht="15">
+    <row r="4" spans="1:6">
       <c r="A4">
         <v>3</v>
       </c>
@@ -970,7 +988,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="5" spans="1:6" ht="15">
+    <row r="5" spans="1:6">
       <c r="A5">
         <v>4</v>
       </c>
@@ -990,7 +1008,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="6" spans="1:6" ht="15">
+    <row r="6" spans="1:6">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1010,7 +1028,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="7" spans="1:6" ht="15">
+    <row r="7" spans="1:6">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1027,7 +1045,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="8" spans="1:6" ht="15">
+    <row r="8" spans="1:6">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1047,7 +1065,7 @@
         <v>121</v>
       </c>
     </row>
-    <row r="9" spans="1:6" ht="15">
+    <row r="9" spans="1:6">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1067,7 +1085,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6" ht="30">
+    <row r="10" spans="1:6" ht="28.5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1087,7 +1105,7 @@
         <v>110</v>
       </c>
     </row>
-    <row r="11" spans="1:6" ht="15">
+    <row r="11" spans="1:6">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1107,7 +1125,7 @@
         <v>129</v>
       </c>
     </row>
-    <row r="12" spans="1:6" ht="15">
+    <row r="12" spans="1:6">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1132,55 +1150,86 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>14</v>
+        <v>151</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
-      <c r="D13" t="s">
-        <v>104</v>
-      </c>
-      <c r="F13" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:6" ht="15">
+    </row>
+    <row r="14" spans="1:6">
       <c r="A14">
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>130</v>
+        <v>154</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>131</v>
+        <v>152</v>
       </c>
       <c r="E14" s="1" t="s">
-        <v>138</v>
+        <v>153</v>
       </c>
       <c r="F14" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="15" spans="1:6" ht="15">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="15" spans="1:6">
       <c r="A15">
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
       <c r="D15" t="s">
+        <v>104</v>
+      </c>
+      <c r="F15" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="16" spans="1:6">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" t="s">
+        <v>130</v>
+      </c>
+      <c r="C16" t="s">
+        <v>3</v>
+      </c>
+      <c r="D16" t="s">
+        <v>131</v>
+      </c>
+      <c r="E16" s="1" t="s">
+        <v>138</v>
+      </c>
+      <c r="F16" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" t="s">
+        <v>13</v>
+      </c>
+      <c r="C17" t="s">
+        <v>3</v>
+      </c>
+      <c r="D17" t="s">
         <v>101</v>
       </c>
-      <c r="E15" t="s">
+      <c r="E17" t="s">
         <v>42</v>
       </c>
-      <c r="F15" t="s">
+      <c r="F17" t="s">
         <v>31</v>
       </c>
     </row>
@@ -1190,7 +1239,8 @@
     <hyperlink ref="E2" r:id="rId2" xr:uid="{A94255E5-8ECE-483E-BE8F-EE9B37DAE260}"/>
     <hyperlink ref="E5" r:id="rId3" xr:uid="{F9808E56-71B8-4EF9-927B-9D68DAE7673D}"/>
     <hyperlink ref="E9" r:id="rId4" xr:uid="{2A6658AF-7FC0-4FB5-9A94-14DD4D416741}"/>
-    <hyperlink ref="E14" r:id="rId5" xr:uid="{D4CFB1C7-1AE1-491B-850A-B6BFAE8BB6A7}"/>
+    <hyperlink ref="E16" r:id="rId5" xr:uid="{D4CFB1C7-1AE1-491B-850A-B6BFAE8BB6A7}"/>
+    <hyperlink ref="E14" r:id="rId6" tooltip="https://www.linkedin.com/in/jjola-unal/" xr:uid="{9B18B642-568C-42D5-8EB7-C9BF52A122A6}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1200,16 +1250,16 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8353AB8B-5FB3-4C2E-B56B-5EAF5DE5DE00}">
   <dimension ref="A1:H3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1303,7 +1353,7 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
chore: add both juans
</commit_message>
<xml_diff>
--- a/public/data/info.xlsx
+++ b/public/data/info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\cisdeli\Purdue\CiampittiLab\ciampitti-lab.github.io\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20F0852F-36AE-4451-95A5-66D0266CD19B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F45EA5-D6AB-49C6-9436-A54AE7033D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13896" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
+    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9960" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="183" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="168">
   <si>
     <t>role</t>
   </si>
@@ -528,6 +528,21 @@
   </si>
   <si>
     <t>I am an agronomist interested in sustainable agriculture and the use of new technologies to improve the yield of agronomic crops. I have hands-on experience in fields crops, data collection, harvesting and pesticides applications, gained through academic projects and internship.</t>
+  </si>
+  <si>
+    <t>juan_fiore.png</t>
+  </si>
+  <si>
+    <t>Juan Douglas</t>
+  </si>
+  <si>
+    <t>juan_douglas.jpg</t>
+  </si>
+  <si>
+    <t>Agronomist graduated from the National University of Córdoba. Focused on digital agriculture with experience in Python and programming for agricultural applications. Areas of contribution include data management, digital tools, and the integration of technology into agricultural systems.</t>
+  </si>
+  <si>
+    <t>Agronomical Engineering undergraduate student from the national university of Colombia, passionate and skilled in fertigation, irrigation, soil physics, and the use of data in agriculture</t>
   </si>
 </sst>
 </file>
@@ -913,10 +928,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EB64B1-8415-484E-B4A1-A632CC3BB222}">
-  <dimension ref="A1:F19"/>
+  <dimension ref="A1:F20"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+      <selection activeCell="F14" sqref="F14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -1171,10 +1186,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>151</v>
+        <v>164</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>165</v>
+      </c>
+      <c r="F13" t="s">
+        <v>167</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1182,19 +1203,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>152</v>
-      </c>
-      <c r="E14" s="1" t="s">
-        <v>153</v>
+        <v>163</v>
       </c>
       <c r="F14" t="s">
-        <v>155</v>
+        <v>166</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1202,16 +1220,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>154</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>104</v>
+        <v>152</v>
+      </c>
+      <c r="E15" s="1" t="s">
+        <v>153</v>
       </c>
       <c r="F15" t="s">
-        <v>32</v>
+        <v>155</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1219,16 +1240,16 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>160</v>
+        <v>14</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>161</v>
+        <v>104</v>
       </c>
       <c r="F16" t="s">
-        <v>162</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1236,19 +1257,16 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>130</v>
+        <v>160</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>131</v>
-      </c>
-      <c r="E17" s="1" t="s">
-        <v>138</v>
+        <v>161</v>
       </c>
       <c r="F17" t="s">
-        <v>132</v>
+        <v>162</v>
       </c>
     </row>
     <row r="18" spans="1:6">
@@ -1256,19 +1274,19 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>13</v>
+        <v>130</v>
       </c>
       <c r="C18" t="s">
         <v>3</v>
       </c>
       <c r="D18" t="s">
-        <v>101</v>
-      </c>
-      <c r="E18" t="s">
-        <v>42</v>
+        <v>131</v>
+      </c>
+      <c r="E18" s="1" t="s">
+        <v>138</v>
       </c>
       <c r="F18" t="s">
-        <v>31</v>
+        <v>132</v>
       </c>
     </row>
     <row r="19" spans="1:6">
@@ -1276,18 +1294,38 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>156</v>
+        <v>13</v>
       </c>
       <c r="C19" t="s">
         <v>3</v>
       </c>
       <c r="D19" t="s">
+        <v>101</v>
+      </c>
+      <c r="E19" t="s">
+        <v>42</v>
+      </c>
+      <c r="F19" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" t="s">
+        <v>156</v>
+      </c>
+      <c r="C20" t="s">
+        <v>3</v>
+      </c>
+      <c r="D20" t="s">
         <v>158</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E20" s="1" t="s">
         <v>159</v>
       </c>
-      <c r="F19" t="s">
+      <c r="F20" t="s">
         <v>157</v>
       </c>
     </row>
@@ -1297,9 +1335,9 @@
     <hyperlink ref="E2" r:id="rId2" xr:uid="{A94255E5-8ECE-483E-BE8F-EE9B37DAE260}"/>
     <hyperlink ref="E5" r:id="rId3" xr:uid="{F9808E56-71B8-4EF9-927B-9D68DAE7673D}"/>
     <hyperlink ref="E9" r:id="rId4" xr:uid="{2A6658AF-7FC0-4FB5-9A94-14DD4D416741}"/>
-    <hyperlink ref="E17" r:id="rId5" xr:uid="{D4CFB1C7-1AE1-491B-850A-B6BFAE8BB6A7}"/>
-    <hyperlink ref="E14" r:id="rId6" tooltip="https://www.linkedin.com/in/jjola-unal/" xr:uid="{9B18B642-568C-42D5-8EB7-C9BF52A122A6}"/>
-    <hyperlink ref="E19" r:id="rId7" xr:uid="{83DA2968-3BAC-44C7-87DD-D7D2815CABF1}"/>
+    <hyperlink ref="E18" r:id="rId5" xr:uid="{D4CFB1C7-1AE1-491B-850A-B6BFAE8BB6A7}"/>
+    <hyperlink ref="E15" r:id="rId6" tooltip="https://www.linkedin.com/in/jjola-unal/" xr:uid="{9B18B642-568C-42D5-8EB7-C9BF52A122A6}"/>
+    <hyperlink ref="E20" r:id="rId7" xr:uid="{83DA2968-3BAC-44C7-87DD-D7D2815CABF1}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
chore: add jd linkedin
</commit_message>
<xml_diff>
--- a/public/data/info.xlsx
+++ b/public/data/info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\cisdeli\Purdue\CiampittiLab\ciampitti-lab.github.io\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34F45EA5-D6AB-49C6-9436-A54AE7033D48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E429D8-5D80-4593-9496-B1082A0BAA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="768" yWindow="768" windowWidth="17280" windowHeight="9960" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
+    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15285" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="168">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="169">
   <si>
     <t>role</t>
   </si>
@@ -543,6 +543,9 @@
   </si>
   <si>
     <t>Agronomical Engineering undergraduate student from the national university of Colombia, passionate and skilled in fertigation, irrigation, soil physics, and the use of data in agriculture</t>
+  </si>
+  <si>
+    <t>https://www.linkedin.com/in/juan-camilo-douglas-bolano-157646293/</t>
   </si>
 </sst>
 </file>
@@ -930,18 +933,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EB64B1-8415-484E-B4A1-A632CC3BB222}">
   <dimension ref="A1:F20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F14" sqref="F14"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="1" max="1" width="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.59765625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.8984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.3984375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="61.3984375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="182.3984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="13.375" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="61.375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="182.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
@@ -1121,7 +1124,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="10" spans="1:6">
+    <row r="10" spans="1:6" ht="28.5">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1193,6 +1196,9 @@
       </c>
       <c r="D13" t="s">
         <v>165</v>
+      </c>
+      <c r="E13" s="1" t="s">
+        <v>168</v>
       </c>
       <c r="F13" t="s">
         <v>167</v>
@@ -1338,6 +1344,7 @@
     <hyperlink ref="E18" r:id="rId5" xr:uid="{D4CFB1C7-1AE1-491B-850A-B6BFAE8BB6A7}"/>
     <hyperlink ref="E15" r:id="rId6" tooltip="https://www.linkedin.com/in/jjola-unal/" xr:uid="{9B18B642-568C-42D5-8EB7-C9BF52A122A6}"/>
     <hyperlink ref="E20" r:id="rId7" xr:uid="{83DA2968-3BAC-44C7-87DD-D7D2815CABF1}"/>
+    <hyperlink ref="E13" r:id="rId8" xr:uid="{C20D33EE-D7E5-4CF8-918D-658532FE0616}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1351,12 +1358,12 @@
       <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
-    <col min="3" max="3" width="11.8984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="13.3984375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="13.375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8">
@@ -1450,7 +1457,7 @@
       <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.8"/>
+  <sheetFormatPr defaultRowHeight="14.25"/>
   <cols>
     <col min="4" max="4" width="30" bestFit="1" customWidth="1"/>
   </cols>

</xml_diff>

<commit_message>
chore: updating team members list
</commit_message>
<xml_diff>
--- a/public/data/info.xlsx
+++ b/public/data/info.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu\home\cisdeli\Purdue\CiampittiLab\ciampitti-lab.github.io\public\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64E429D8-5D80-4593-9496-B1082A0BAA19}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD7D56A7-DBBB-421C-9B21-E90A98FDE59D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3510" yWindow="3510" windowWidth="28800" windowHeight="15285" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{680A29BD-E113-4DFE-A325-D924D35BBF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="team" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="190" uniqueCount="169">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="157">
   <si>
     <t>role</t>
   </si>
@@ -393,42 +393,6 @@
   </si>
   <si>
     <t>Agronomist researching sustainable corn-soybean systems, using digital tools to assess how crop rotation, cover crops, and nitrogen management impact soil health, environmental resilience, and overall farm productivity and profitability.</t>
-  </si>
-  <si>
-    <t>francisco_palmero.jpg</t>
-  </si>
-  <si>
-    <t>Francisco Palmero</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/francisco-palmero-6b8826170/</t>
-  </si>
-  <si>
-    <t>Focuses on applied statistics for agriculture-related problems, with emphasis on nitrogen management and corn physiology. Background in the role of legume crops in soil nitrogen budgets within agricultural systems.</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/diogo-verzegnazzi-555418239/</t>
-  </si>
-  <si>
-    <t>Diogo Verzegnazzi</t>
-  </si>
-  <si>
-    <t>diogo_verzegnazzi.jpg</t>
-  </si>
-  <si>
-    <t>Caetano Rocha</t>
-  </si>
-  <si>
-    <t>caetano_rocha.jpg</t>
-  </si>
-  <si>
-    <t>https://www.linkedin.com/in/caetano-rocha-9087b0319/</t>
-  </si>
-  <si>
-    <t>Agronomy undergraduate from University of Santa Maria with experience in field crops. Supports field operations through crop monitoring, data collection, and hands-on agricultural practices across research sites.</t>
-  </si>
-  <si>
-    <t>Agronomy undergraduate from University of Santa Maria with experience in field crops and soil science. Supports field operations through crop monitoring, data collection, and hands-on agricultural practices across research sites.</t>
   </si>
   <si>
     <t>Roberto Romero</t>
@@ -931,10 +895,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{87EB64B1-8415-484E-B4A1-A632CC3BB222}">
-  <dimension ref="A1:F20"/>
+  <dimension ref="A1:F17"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E25" sqref="E25"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.25"/>
@@ -1089,59 +1053,59 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>119</v>
+        <v>12</v>
       </c>
       <c r="C8" t="s">
         <v>26</v>
       </c>
       <c r="D8" t="s">
-        <v>118</v>
+        <v>102</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>120</v>
+        <v>40</v>
       </c>
       <c r="F8" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="9" spans="1:6">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="9" spans="1:6" ht="28.5">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" t="s">
         <v>26</v>
       </c>
       <c r="D9" t="s">
-        <v>102</v>
+        <v>107</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="F9" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="10" spans="1:6" ht="28.5">
+        <v>41</v>
+      </c>
+      <c r="F9" s="2" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="10" spans="1:6">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>10</v>
+        <v>152</v>
       </c>
       <c r="C10" t="s">
-        <v>26</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>107</v>
+        <v>153</v>
       </c>
       <c r="E10" s="1" t="s">
-        <v>41</v>
-      </c>
-      <c r="F10" s="2" t="s">
-        <v>110</v>
+        <v>156</v>
+      </c>
+      <c r="F10" t="s">
+        <v>155</v>
       </c>
     </row>
     <row r="11" spans="1:6">
@@ -1149,19 +1113,16 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>125</v>
+        <v>139</v>
       </c>
       <c r="C11" t="s">
         <v>3</v>
       </c>
       <c r="D11" t="s">
-        <v>126</v>
-      </c>
-      <c r="E11" t="s">
-        <v>127</v>
+        <v>151</v>
       </c>
       <c r="F11" t="s">
-        <v>129</v>
+        <v>154</v>
       </c>
     </row>
     <row r="12" spans="1:6">
@@ -1169,19 +1130,19 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>123</v>
+        <v>142</v>
       </c>
       <c r="C12" t="s">
         <v>3</v>
       </c>
       <c r="D12" t="s">
-        <v>124</v>
-      </c>
-      <c r="E12" t="s">
-        <v>122</v>
+        <v>140</v>
+      </c>
+      <c r="E12" s="1" t="s">
+        <v>141</v>
       </c>
       <c r="F12" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
     </row>
     <row r="13" spans="1:6">
@@ -1189,19 +1150,16 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>164</v>
+        <v>14</v>
       </c>
       <c r="C13" t="s">
         <v>3</v>
       </c>
       <c r="D13" t="s">
-        <v>165</v>
-      </c>
-      <c r="E13" s="1" t="s">
-        <v>168</v>
+        <v>104</v>
       </c>
       <c r="F13" t="s">
-        <v>167</v>
+        <v>32</v>
       </c>
     </row>
     <row r="14" spans="1:6">
@@ -1209,16 +1167,16 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="C14" t="s">
         <v>3</v>
       </c>
       <c r="D14" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
       <c r="F14" t="s">
-        <v>166</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:6">
@@ -1226,19 +1184,19 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>154</v>
+        <v>118</v>
       </c>
       <c r="C15" t="s">
         <v>3</v>
       </c>
       <c r="D15" t="s">
-        <v>152</v>
+        <v>119</v>
       </c>
       <c r="E15" s="1" t="s">
-        <v>153</v>
+        <v>126</v>
       </c>
       <c r="F15" t="s">
-        <v>155</v>
+        <v>120</v>
       </c>
     </row>
     <row r="16" spans="1:6">
@@ -1246,16 +1204,19 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" t="s">
         <v>3</v>
       </c>
       <c r="D16" t="s">
-        <v>104</v>
+        <v>101</v>
+      </c>
+      <c r="E16" t="s">
+        <v>42</v>
       </c>
       <c r="F16" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="17" spans="1:6">
@@ -1263,76 +1224,19 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>160</v>
+        <v>144</v>
       </c>
       <c r="C17" t="s">
         <v>3</v>
       </c>
       <c r="D17" t="s">
-        <v>161</v>
+        <v>146</v>
+      </c>
+      <c r="E17" s="1" t="s">
+        <v>147</v>
       </c>
       <c r="F17" t="s">
-        <v>162</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6">
-      <c r="A18">
-        <v>17</v>
-      </c>
-      <c r="B18" t="s">
-        <v>130</v>
-      </c>
-      <c r="C18" t="s">
-        <v>3</v>
-      </c>
-      <c r="D18" t="s">
-        <v>131</v>
-      </c>
-      <c r="E18" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F18" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6">
-      <c r="A19">
-        <v>18</v>
-      </c>
-      <c r="B19" t="s">
-        <v>13</v>
-      </c>
-      <c r="C19" t="s">
-        <v>3</v>
-      </c>
-      <c r="D19" t="s">
-        <v>101</v>
-      </c>
-      <c r="E19" t="s">
-        <v>42</v>
-      </c>
-      <c r="F19" t="s">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6">
-      <c r="A20">
-        <v>19</v>
-      </c>
-      <c r="B20" t="s">
-        <v>156</v>
-      </c>
-      <c r="C20" t="s">
-        <v>3</v>
-      </c>
-      <c r="D20" t="s">
-        <v>158</v>
-      </c>
-      <c r="E20" s="1" t="s">
-        <v>159</v>
-      </c>
-      <c r="F20" t="s">
-        <v>157</v>
+        <v>145</v>
       </c>
     </row>
   </sheetData>
@@ -1340,11 +1244,11 @@
     <hyperlink ref="E3" r:id="rId1" xr:uid="{AAA55F43-9F3C-40DB-9B47-46AAC432FF09}"/>
     <hyperlink ref="E2" r:id="rId2" xr:uid="{A94255E5-8ECE-483E-BE8F-EE9B37DAE260}"/>
     <hyperlink ref="E5" r:id="rId3" xr:uid="{F9808E56-71B8-4EF9-927B-9D68DAE7673D}"/>
-    <hyperlink ref="E9" r:id="rId4" xr:uid="{2A6658AF-7FC0-4FB5-9A94-14DD4D416741}"/>
-    <hyperlink ref="E18" r:id="rId5" xr:uid="{D4CFB1C7-1AE1-491B-850A-B6BFAE8BB6A7}"/>
-    <hyperlink ref="E15" r:id="rId6" tooltip="https://www.linkedin.com/in/jjola-unal/" xr:uid="{9B18B642-568C-42D5-8EB7-C9BF52A122A6}"/>
-    <hyperlink ref="E20" r:id="rId7" xr:uid="{83DA2968-3BAC-44C7-87DD-D7D2815CABF1}"/>
-    <hyperlink ref="E13" r:id="rId8" xr:uid="{C20D33EE-D7E5-4CF8-918D-658532FE0616}"/>
+    <hyperlink ref="E8" r:id="rId4" xr:uid="{2A6658AF-7FC0-4FB5-9A94-14DD4D416741}"/>
+    <hyperlink ref="E15" r:id="rId5" xr:uid="{D4CFB1C7-1AE1-491B-850A-B6BFAE8BB6A7}"/>
+    <hyperlink ref="E12" r:id="rId6" tooltip="https://www.linkedin.com/in/jjola-unal/" xr:uid="{9B18B642-568C-42D5-8EB7-C9BF52A122A6}"/>
+    <hyperlink ref="E17" r:id="rId7" xr:uid="{83DA2968-3BAC-44C7-87DD-D7D2815CABF1}"/>
+    <hyperlink ref="E10" r:id="rId8" xr:uid="{C20D33EE-D7E5-4CF8-918D-658532FE0616}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -1374,7 +1278,7 @@
         <v>17</v>
       </c>
       <c r="C1" t="s">
-        <v>143</v>
+        <v>131</v>
       </c>
       <c r="D1" t="s">
         <v>18</v>
@@ -1400,7 +1304,7 @@
         <v>114</v>
       </c>
       <c r="C2" t="s">
-        <v>144</v>
+        <v>132</v>
       </c>
       <c r="D2" t="s">
         <v>113</v>
@@ -1423,25 +1327,25 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>137</v>
       </c>
       <c r="C3" t="s">
-        <v>145</v>
+        <v>133</v>
       </c>
       <c r="D3" t="s">
-        <v>150</v>
+        <v>138</v>
       </c>
       <c r="E3" t="s">
-        <v>146</v>
+        <v>134</v>
       </c>
       <c r="F3" t="s">
         <v>115</v>
       </c>
       <c r="G3" t="s">
-        <v>147</v>
+        <v>135</v>
       </c>
       <c r="H3" t="s">
-        <v>148</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -1743,22 +1647,22 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>133</v>
+        <v>121</v>
       </c>
       <c r="C13" t="s">
-        <v>134</v>
+        <v>122</v>
       </c>
       <c r="D13" t="s">
-        <v>135</v>
+        <v>123</v>
       </c>
       <c r="E13">
         <v>2025</v>
       </c>
       <c r="F13" t="s">
-        <v>136</v>
+        <v>124</v>
       </c>
       <c r="G13" t="s">
-        <v>137</v>
+        <v>125</v>
       </c>
     </row>
     <row r="14" spans="1:7">
@@ -1766,19 +1670,19 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>139</v>
+        <v>127</v>
       </c>
       <c r="C14" t="s">
-        <v>140</v>
+        <v>128</v>
       </c>
       <c r="D14" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
       <c r="E14">
         <v>2025</v>
       </c>
       <c r="F14" s="1" t="s">
-        <v>141</v>
+        <v>129</v>
       </c>
       <c r="G14" s="1"/>
     </row>

</xml_diff>